<commit_message>
sept 4 core business TC1-12
</commit_message>
<xml_diff>
--- a/src/test/resources/Testdata/data.xlsx
+++ b/src/test/resources/Testdata/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="5" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,13 +15,15 @@
     <sheet name="no email no name" sheetId="8" r:id="rId6"/>
     <sheet name="no name valid email" sheetId="9" r:id="rId7"/>
     <sheet name="valid name invalid email" sheetId="10" r:id="rId8"/>
+    <sheet name="Login invalid Credentials" sheetId="11" r:id="rId9"/>
+    <sheet name="Login valid Credentials" sheetId="12" r:id="rId10"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>jaikrishnaa</t>
   </si>
@@ -60,6 +62,15 @@
   </si>
   <si>
     <t>jiak@p</t>
+  </si>
+  <si>
+    <t>jaikrishnagit@gmail.com</t>
+  </si>
+  <si>
+    <t>Team@A8</t>
+  </si>
+  <si>
+    <t>Team@A23</t>
   </si>
 </sst>
 </file>
@@ -437,6 +448,37 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.5546875" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1"/>
+    <hyperlink ref="B1" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
@@ -617,7 +659,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -640,4 +682,35 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="34.5546875" customWidth="1"/>
+    <col min="2" max="2" width="14.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1"/>
+    <hyperlink ref="B1" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
New update in testng.xml
</commit_message>
<xml_diff>
--- a/src/test/resources/Testdata/data.xlsx
+++ b/src/test/resources/Testdata/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="5" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="2436" windowWidth="17400" windowHeight="8076" firstSheet="6" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="Login invalid Credentials" sheetId="11" r:id="rId9"/>
     <sheet name="Login valid Credentials" sheetId="12" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:O26"/>
 </workbook>
 </file>
 

</xml_diff>